<commit_message>
changed binary cost files to €/g
</commit_message>
<xml_diff>
--- a/data/cost_format/Cost_PLA.xlsx
+++ b/data/cost_format/Cost_PLA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/cost_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B4CD8A-880A-2746-99CB-8C956905EACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DA84E3-B087-6E4F-97D0-2B63A12B0ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8240" yWindow="500" windowWidth="25360" windowHeight="17400" activeTab="1" xr2:uid="{968F1003-936B-E54A-97BA-F1A20154874A}"/>
+    <workbookView xWindow="8240" yWindow="500" windowWidth="25360" windowHeight="17400" xr2:uid="{968F1003-936B-E54A-97BA-F1A20154874A}"/>
   </bookViews>
   <sheets>
     <sheet name="economical_params" sheetId="1" r:id="rId1"/>
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D55A5A-B7EB-8045-ACFE-203E25D14010}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,7 +481,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="5">
-        <v>34.9</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -512,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B71B34F-5162-EF46-8C76-5B2F32AD0283}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -538,11 +538,11 @@
       </c>
       <c r="B2" s="7">
         <f>economical_params!B2*0.8</f>
-        <v>27.92</v>
+        <v>2.8000000000000004E-2</v>
       </c>
       <c r="C2" s="7">
         <f>economical_params!B2*2</f>
-        <v>69.8</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D2" s="7">
         <v>1</v>

</xml_diff>